<commit_message>
game length by ELO difference
</commit_message>
<xml_diff>
--- a/wins_by_difference.xlsx
+++ b/wins_by_difference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="11475" windowHeight="6480" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="11475" windowHeight="6480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>higher wins</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>survival:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total </t>
+  </si>
+  <si>
+    <t>Moves</t>
   </si>
 </sst>
 </file>
@@ -640,11 +646,11 @@
         </c:ser>
         <c:gapWidth val="135"/>
         <c:overlap val="100"/>
-        <c:axId val="175647744"/>
-        <c:axId val="190206720"/>
+        <c:axId val="168032512"/>
+        <c:axId val="168050688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175647744"/>
+        <c:axId val="168032512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +658,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190206720"/>
+        <c:crossAx val="168050688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -660,7 +666,7 @@
         <c:tickLblSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190206720"/>
+        <c:axId val="168050688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +675,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175647744"/>
+        <c:crossAx val="168032512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -683,7 +689,174 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$D$3:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$3:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>76.058823529411697</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.369230769230697</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.199218749999901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.514018691588703</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.7899022801302</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.035143769968002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.322857142857103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41.034482758620598</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.233009708737796</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.474074074073997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.212121212121197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35.813333333333297</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="37243520"/>
+        <c:axId val="37258368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="37243520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37258368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="2"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37258368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37243520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -703,6 +876,41 @@
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1009,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E2:J42"/>
+  <dimension ref="C2:J42"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1024,7 +1232,10 @@
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:10">
+    <row r="2" spans="3:10">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
@@ -1038,7 +1249,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="5:10">
+    <row r="3" spans="3:10">
+      <c r="C3">
+        <f>H3+I3+J3</f>
+        <v>34</v>
+      </c>
       <c r="E3">
         <v>0</v>
       </c>
@@ -1055,7 +1270,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="5:10">
+    <row r="4" spans="3:10">
+      <c r="C4">
+        <f t="shared" ref="C4:C24" si="0">H4+I4+J4</f>
+        <v>65</v>
+      </c>
       <c r="E4">
         <f>E3+50</f>
         <v>50</v>
@@ -1074,13 +1293,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="5:10">
+    <row r="5" spans="3:10">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
       <c r="E5">
-        <f t="shared" ref="E5:E24" si="0">E4+50</f>
+        <f t="shared" ref="E5:E24" si="1">E4+50</f>
         <v>100</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F24" si="1">F4+50</f>
+        <f t="shared" ref="F5:F24" si="2">F4+50</f>
         <v>149</v>
       </c>
       <c r="H5">
@@ -1093,13 +1316,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="5:10">
+    <row r="6" spans="3:10">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>535</v>
+      </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>199</v>
       </c>
       <c r="H6">
@@ -1112,13 +1339,17 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="5:10">
+    <row r="7" spans="3:10">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>614</v>
+      </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>249</v>
       </c>
       <c r="H7">
@@ -1131,13 +1362,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="5:10">
+    <row r="8" spans="3:10">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>626</v>
+      </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>299</v>
       </c>
       <c r="H8">
@@ -1150,13 +1385,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="5:10">
+    <row r="9" spans="3:10">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>349</v>
       </c>
       <c r="H9">
@@ -1169,13 +1408,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="5:10">
+    <row r="10" spans="3:10">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>399</v>
       </c>
       <c r="H10">
@@ -1188,13 +1431,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="5:10">
+    <row r="11" spans="3:10">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>449</v>
       </c>
       <c r="H11">
@@ -1207,13 +1454,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="5:10">
+    <row r="12" spans="3:10">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>450</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>499</v>
       </c>
       <c r="H12">
@@ -1226,13 +1477,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="5:10">
+    <row r="13" spans="3:10">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>549</v>
       </c>
       <c r="H13">
@@ -1245,13 +1500,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="5:10">
+    <row r="14" spans="3:10">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>550</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>599</v>
       </c>
       <c r="H14">
@@ -1264,13 +1523,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="5:10">
+    <row r="15" spans="3:10">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>649</v>
       </c>
       <c r="H15">
@@ -1283,13 +1546,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="5:10">
+    <row r="16" spans="3:10">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>650</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>699</v>
       </c>
       <c r="H16">
@@ -1302,13 +1569,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="5:10">
+    <row r="17" spans="3:10">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>700</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>749</v>
       </c>
       <c r="H17">
@@ -1321,13 +1592,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="5:10">
+    <row r="18" spans="3:10">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>750</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>799</v>
       </c>
       <c r="H18">
@@ -1340,13 +1615,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="5:10">
+    <row r="19" spans="3:10">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>849</v>
       </c>
       <c r="H19">
@@ -1359,13 +1638,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="5:10">
+    <row r="20" spans="3:10">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>850</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>899</v>
       </c>
       <c r="H20">
@@ -1378,13 +1661,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="3:10">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>949</v>
       </c>
       <c r="H21">
@@ -1397,13 +1684,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="3:10">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>950</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>999</v>
       </c>
       <c r="H22">
@@ -1416,13 +1707,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="3:10">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1049</v>
       </c>
       <c r="H23">
@@ -1435,13 +1730,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="3:10">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1050</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1099</v>
       </c>
       <c r="H24">
@@ -1454,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="3:10">
       <c r="H25">
         <v>0</v>
       </c>
@@ -1465,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="3:10">
       <c r="H26">
         <v>0</v>
       </c>
@@ -1476,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="3:10">
       <c r="H27">
         <v>0</v>
       </c>
@@ -1487,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="3:10">
       <c r="H28">
         <v>0</v>
       </c>
@@ -1498,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="3:10">
       <c r="H29">
         <v>0</v>
       </c>
@@ -1509,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="3:10">
       <c r="H30">
         <v>0</v>
       </c>
@@ -1520,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="3:10">
       <c r="H31">
         <v>0</v>
       </c>
@@ -1531,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="3:10">
       <c r="H32">
         <v>0</v>
       </c>
@@ -1662,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1675,6 +1974,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="K2">
+        <v>3258</v>
+      </c>
     </row>
     <row r="3" spans="2:20">
       <c r="B3">
@@ -2119,26 +2421,28 @@
         <v>15</v>
       </c>
       <c r="M12">
-        <f>2*6851</f>
-        <v>13702</v>
+        <f>4*$K$2</f>
+        <v>13032</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:O12" si="3">2*6851</f>
-        <v>13702</v>
+        <f>4*$K$2</f>
+        <v>13032</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
-        <v>13702</v>
+        <f>4*$K$2</f>
+        <v>13032</v>
       </c>
       <c r="P12">
-        <v>6851</v>
+        <f>2*$K$2</f>
+        <v>6516</v>
       </c>
       <c r="Q12">
-        <v>6851</v>
+        <f>2*$K$2</f>
+        <v>6516</v>
       </c>
       <c r="R12">
-        <f>8*6851</f>
-        <v>54808</v>
+        <f>16*$K$2</f>
+        <v>52128</v>
       </c>
     </row>
     <row r="13" spans="2:20">
@@ -2150,27 +2454,27 @@
       </c>
       <c r="M13">
         <f>1 - M11/M12</f>
-        <v>0.54189169464311782</v>
+        <v>0.51833947206875386</v>
       </c>
       <c r="N13">
-        <f t="shared" ref="N13:R13" si="4">1 - N11/N12</f>
-        <v>0.2730258356444315</v>
+        <f t="shared" ref="N13:R13" si="3">1 - N11/N12</f>
+        <v>0.23565070595457338</v>
       </c>
       <c r="O13">
-        <f t="shared" si="4"/>
-        <v>0.34724857685009491</v>
+        <f t="shared" si="3"/>
+        <v>0.31368937998772251</v>
       </c>
       <c r="P13">
-        <f t="shared" si="4"/>
-        <v>0.47715661947161003</v>
+        <f t="shared" si="3"/>
+        <v>0.45027624309392267</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R13">
-        <f t="shared" si="4"/>
-        <v>0.54608816231207125</v>
+        <f t="shared" si="3"/>
+        <v>0.52275168815224071</v>
       </c>
     </row>
     <row r="14" spans="2:20">
@@ -2424,12 +2728,377 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>76.058823529411697</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <f>A3*50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>68.369230769230697</v>
+      </c>
+      <c r="C4">
+        <v>65</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D24" si="0">A4*50</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <f>1+A4</f>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>60.199218749999901</v>
+      </c>
+      <c r="C5">
+        <v>256</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <f t="shared" ref="A6:A24" si="1">1+A5</f>
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>49.514018691588703</v>
+      </c>
+      <c r="C6">
+        <v>535</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>47.7899022801302</v>
+      </c>
+      <c r="C7">
+        <v>614</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>43.035143769968002</v>
+      </c>
+      <c r="C8">
+        <v>626</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>43.322857142857103</v>
+      </c>
+      <c r="C9">
+        <v>350</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>41.034482758620598</v>
+      </c>
+      <c r="C10">
+        <v>174</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>39.233009708737796</v>
+      </c>
+      <c r="C11">
+        <v>103</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>39.474074074073997</v>
+      </c>
+      <c r="C12">
+        <v>135</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>36.212121212121197</v>
+      </c>
+      <c r="C13">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>35.813333333333297</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>39.076923076923002</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>35.4</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>34.692307692307601</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>36.6666666666666</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>26.3333333333333</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="C25">
+        <f>SUM(C3:C24)</f>
+        <v>3251</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>